<commit_message>
Progetto linguaggi a, candidato parser
</commit_message>
<xml_diff>
--- a/Bruniera/linguaggi e compilatori/progetto/parteA/tabella2.xlsx
+++ b/Bruniera/linguaggi e compilatori/progetto/parteA/tabella2.xlsx
@@ -13,7 +13,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+  <si>
+    <t>NT\la</t>
+  </si>
   <si>
     <t>(</t>
   </si>
@@ -268,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -278,6 +281,11 @@
     <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="0" fillId="0" borderId="1" numFmtId="0" xfId="0" applyBorder="1"/>
     <xf fontId="4" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -786,7 +794,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="100" workbookViewId="0">
+    <sheetView zoomScale="100" workbookViewId="0">
       <selection activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -797,50 +805,52 @@
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="18.75">
-      <c r="A1" s="2"/>
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" ht="14.25">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="4">
         <v>2</v>
@@ -876,7 +886,7 @@
         <v>2</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="N2" s="4">
         <v>1</v>
@@ -884,7 +894,7 @@
     </row>
     <row r="3" ht="14.25">
       <c r="A3" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B3" s="4">
         <v>3</v>
@@ -908,13 +918,13 @@
         <v>10</v>
       </c>
       <c r="I3" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J3" s="4">
         <v>12</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="L3" s="6">
         <v>10</v>
@@ -928,19 +938,19 @@
     </row>
     <row r="4" ht="14.25">
       <c r="A4" s="3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B4" s="4">
         <v>3</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D4" s="4">
         <v>4</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F4" s="4">
         <v>6</v>
@@ -949,7 +959,7 @@
         <v>6</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I4" s="4">
         <v>11</v>
@@ -961,18 +971,18 @@
         <v>11</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="M4" s="4">
         <v>6</v>
       </c>
       <c r="N4" s="7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B5" s="4">
         <v>2</v>
@@ -996,19 +1006,19 @@
         <v>2</v>
       </c>
       <c r="I5" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J5" s="4">
         <v>2</v>
       </c>
       <c r="K5" s="5" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="L5" s="4">
         <v>2</v>
       </c>
       <c r="M5" s="5" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N5" s="4">
         <v>1</v>
@@ -1016,7 +1026,7 @@
     </row>
     <row r="6" ht="14.25">
       <c r="A6" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B6" s="4">
         <v>3</v>
@@ -1031,10 +1041,10 @@
         <v>3</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H6" s="4">
         <v>8</v>
@@ -1060,7 +1070,7 @@
     </row>
     <row r="7" ht="14.25">
       <c r="A7" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B7" s="4">
         <v>3</v>
@@ -1084,13 +1094,13 @@
         <v>16</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J7" s="4">
         <v>3</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L7" s="4">
         <v>16</v>
@@ -1104,28 +1114,28 @@
     </row>
     <row r="8" ht="14.25">
       <c r="A8" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B8" s="4">
         <v>3</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="5" t="s">
-        <v>31</v>
-      </c>
       <c r="F8" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="I8" s="4">
         <v>15</v>
@@ -1137,21 +1147,21 @@
         <v>15</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="M8" s="4">
         <v>3</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" ht="14.25">
       <c r="A9" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C9" s="4">
         <v>3</v>
@@ -1172,19 +1182,19 @@
         <v>7</v>
       </c>
       <c r="I9" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J9" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="K9" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="K9" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="L9" s="4">
         <v>7</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="N9" s="4">
         <v>1</v>
@@ -1192,7 +1202,7 @@
     </row>
     <row r="10" ht="14.25">
       <c r="A10" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B10" s="4">
         <v>19</v>
@@ -1213,7 +1223,7 @@
         <v>19</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="I10" s="4">
         <v>19</v>
@@ -1225,7 +1235,7 @@
         <v>19</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="M10" s="4">
         <v>19</v>
@@ -1239,160 +1249,489 @@
     <row r="13" ht="14.25"/>
     <row r="14" ht="14.25">
       <c r="A14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" ht="14.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" ht="15.6" customHeight="1">
       <c r="A15" s="6">
         <v>1</v>
       </c>
-      <c r="B15" t="s">
-        <v>41</v>
-      </c>
+      <c r="B15" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="9"/>
+      <c r="K15" s="10"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
+      <c r="N15" s="11"/>
+      <c r="O15" s="11"/>
+      <c r="P15" s="11"/>
+      <c r="Q15" s="11"/>
+      <c r="R15" s="11"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11"/>
+      <c r="U15" s="11"/>
+      <c r="V15" s="11"/>
+      <c r="W15" s="11"/>
+      <c r="X15" s="11"/>
     </row>
     <row r="16" ht="14.25">
       <c r="A16" s="6">
         <v>2</v>
       </c>
-      <c r="B16" t="s">
-        <v>42</v>
-      </c>
+      <c r="B16" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="9"/>
+      <c r="K16" s="10"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="13"/>
+      <c r="N16" s="13"/>
+      <c r="O16" s="13"/>
+      <c r="P16" s="13"/>
+      <c r="Q16" s="13"/>
+      <c r="R16" s="13"/>
+      <c r="S16" s="13"/>
+      <c r="T16" s="13"/>
+      <c r="U16" s="13"/>
+      <c r="V16" s="13"/>
+      <c r="W16" s="13"/>
+      <c r="X16" s="13"/>
     </row>
     <row r="17" ht="14.25">
       <c r="A17" s="6">
         <v>3</v>
       </c>
-      <c r="B17" t="s">
-        <v>43</v>
-      </c>
+      <c r="B17" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="13"/>
+      <c r="O17" s="13"/>
+      <c r="P17" s="13"/>
+      <c r="Q17" s="13"/>
+      <c r="R17" s="13"/>
+      <c r="S17" s="13"/>
+      <c r="T17" s="13"/>
+      <c r="U17" s="13"/>
+      <c r="V17" s="13"/>
+      <c r="W17" s="13"/>
+      <c r="X17" s="13"/>
     </row>
     <row r="18" ht="14.25">
       <c r="A18" s="6">
         <v>4</v>
       </c>
-      <c r="B18" t="s">
-        <v>44</v>
-      </c>
+      <c r="B18" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="K18" s="10"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="13"/>
+      <c r="P18" s="13"/>
+      <c r="Q18" s="13"/>
+      <c r="R18" s="13"/>
+      <c r="S18" s="13"/>
+      <c r="T18" s="13"/>
+      <c r="U18" s="13"/>
+      <c r="V18" s="13"/>
+      <c r="W18" s="13"/>
+      <c r="X18" s="13"/>
     </row>
     <row r="19" ht="14.25">
       <c r="A19" s="6">
         <v>5</v>
       </c>
-      <c r="B19" t="s">
-        <v>45</v>
-      </c>
+      <c r="B19" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="K19" s="10"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="12"/>
+      <c r="P19" s="13"/>
+      <c r="Q19" s="13"/>
+      <c r="R19" s="13"/>
+      <c r="S19" s="13"/>
+      <c r="T19" s="13"/>
+      <c r="U19" s="13"/>
+      <c r="V19" s="13"/>
+      <c r="W19" s="13"/>
+      <c r="X19" s="13"/>
     </row>
     <row r="20" ht="14.25">
       <c r="A20" s="6">
         <v>6</v>
       </c>
-      <c r="B20" t="s">
-        <v>46</v>
-      </c>
+      <c r="B20" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="K20" s="10"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="13"/>
+      <c r="N20" s="13"/>
+      <c r="O20" s="13"/>
+      <c r="P20" s="12"/>
+      <c r="Q20" s="13"/>
+      <c r="R20" s="13"/>
+      <c r="S20" s="13"/>
+      <c r="T20" s="13"/>
+      <c r="U20" s="13"/>
+      <c r="V20" s="13"/>
+      <c r="W20" s="13"/>
+      <c r="X20" s="13"/>
     </row>
     <row r="21" ht="14.25">
       <c r="A21" s="6">
         <v>7</v>
       </c>
-      <c r="B21" s="9" t="s">
-        <v>47</v>
-      </c>
+      <c r="B21" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="K21" s="10"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="13"/>
+      <c r="N21" s="13"/>
+      <c r="O21" s="13"/>
+      <c r="P21" s="13"/>
+      <c r="Q21" s="12"/>
+      <c r="R21" s="13"/>
+      <c r="S21" s="13"/>
+      <c r="T21" s="13"/>
+      <c r="U21" s="13"/>
+      <c r="V21" s="13"/>
+      <c r="W21" s="13"/>
+      <c r="X21" s="13"/>
     </row>
     <row r="22" ht="14.25">
       <c r="A22" s="6">
         <v>8</v>
       </c>
-      <c r="B22" t="s">
-        <v>48</v>
-      </c>
+      <c r="B22" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="K22" s="10"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="13"/>
+      <c r="R22" s="12"/>
+      <c r="S22" s="13"/>
+      <c r="T22" s="13"/>
+      <c r="U22" s="13"/>
+      <c r="V22" s="13"/>
+      <c r="W22" s="13"/>
+      <c r="X22" s="13"/>
     </row>
     <row r="23" ht="14.25">
       <c r="A23" s="6">
         <v>9</v>
       </c>
-      <c r="B23" t="s">
-        <v>49</v>
-      </c>
+      <c r="B23" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="K23" s="10"/>
+      <c r="L23" s="13"/>
+      <c r="M23" s="13"/>
+      <c r="N23" s="13"/>
+      <c r="O23" s="13"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="13"/>
+      <c r="R23" s="13"/>
+      <c r="S23" s="12"/>
+      <c r="T23" s="13"/>
+      <c r="U23" s="13"/>
+      <c r="V23" s="13"/>
+      <c r="W23" s="13"/>
+      <c r="X23" s="13"/>
     </row>
     <row r="24" ht="14.25">
       <c r="A24" s="6">
         <v>10</v>
       </c>
-      <c r="B24" t="s">
-        <v>50</v>
-      </c>
+      <c r="B24" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="K24" s="10"/>
+      <c r="L24" s="13"/>
+      <c r="M24" s="13"/>
+      <c r="N24" s="13"/>
+      <c r="O24" s="13"/>
+      <c r="P24" s="13"/>
+      <c r="Q24" s="13"/>
+      <c r="R24" s="13"/>
+      <c r="S24" s="13"/>
+      <c r="T24" s="12"/>
+      <c r="U24" s="13"/>
+      <c r="V24" s="13"/>
+      <c r="W24" s="13"/>
+      <c r="X24" s="13"/>
     </row>
     <row r="25" ht="14.25">
       <c r="A25" s="6">
         <v>11</v>
       </c>
-      <c r="B25" t="s">
-        <v>51</v>
-      </c>
+      <c r="B25" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="9"/>
+      <c r="K25" s="10"/>
+      <c r="L25" s="13"/>
+      <c r="M25" s="13"/>
+      <c r="N25" s="13"/>
+      <c r="O25" s="13"/>
+      <c r="P25" s="13"/>
+      <c r="Q25" s="13"/>
+      <c r="R25" s="13"/>
+      <c r="S25" s="13"/>
+      <c r="T25" s="13"/>
+      <c r="U25" s="12"/>
+      <c r="V25" s="13"/>
+      <c r="W25" s="13"/>
+      <c r="X25" s="13"/>
     </row>
     <row r="26" ht="14.25">
       <c r="A26" s="6">
         <v>12</v>
       </c>
-      <c r="B26" t="s">
-        <v>52</v>
-      </c>
+      <c r="B26" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
+      <c r="G26" s="9"/>
+      <c r="H26" s="9"/>
+      <c r="I26" s="9"/>
+      <c r="K26" s="10"/>
+      <c r="L26" s="13"/>
+      <c r="M26" s="13"/>
+      <c r="N26" s="13"/>
+      <c r="O26" s="13"/>
+      <c r="P26" s="13"/>
+      <c r="Q26" s="13"/>
+      <c r="R26" s="13"/>
+      <c r="S26" s="13"/>
+      <c r="T26" s="13"/>
+      <c r="U26" s="13"/>
+      <c r="V26" s="12"/>
+      <c r="W26" s="13"/>
+      <c r="X26" s="13"/>
     </row>
     <row r="27" ht="14.25">
       <c r="A27" s="6">
         <v>13</v>
       </c>
-      <c r="B27" t="s">
-        <v>53</v>
-      </c>
+      <c r="B27" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="9"/>
+      <c r="K27" s="10"/>
+      <c r="L27" s="13"/>
+      <c r="M27" s="13"/>
+      <c r="N27" s="13"/>
+      <c r="O27" s="13"/>
+      <c r="P27" s="13"/>
+      <c r="Q27" s="13"/>
+      <c r="R27" s="13"/>
+      <c r="S27" s="13"/>
+      <c r="T27" s="13"/>
+      <c r="U27" s="13"/>
+      <c r="V27" s="13"/>
+      <c r="W27" s="12"/>
+      <c r="X27" s="13"/>
     </row>
     <row r="28" ht="14.25">
       <c r="A28" s="6">
         <v>14</v>
       </c>
-      <c r="B28" t="s">
-        <v>54</v>
-      </c>
+      <c r="B28" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="9"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="9"/>
+      <c r="K28" s="10"/>
+      <c r="L28" s="13"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="13"/>
+      <c r="O28" s="13"/>
+      <c r="P28" s="13"/>
+      <c r="Q28" s="13"/>
+      <c r="R28" s="13"/>
+      <c r="S28" s="13"/>
+      <c r="T28" s="13"/>
+      <c r="U28" s="13"/>
+      <c r="V28" s="13"/>
+      <c r="W28" s="13"/>
+      <c r="X28" s="12"/>
     </row>
     <row r="29" ht="14.25">
       <c r="A29" s="6">
         <v>15</v>
       </c>
-      <c r="B29" t="s">
-        <v>55</v>
-      </c>
+      <c r="B29" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
     </row>
     <row r="30" ht="14.25">
       <c r="A30" s="6">
         <v>16</v>
       </c>
-      <c r="B30" t="s">
-        <v>56</v>
-      </c>
+      <c r="B30" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="9"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
     </row>
     <row r="31" ht="14.25">
       <c r="A31" s="6">
         <v>17</v>
       </c>
-      <c r="B31" t="s">
-        <v>57</v>
-      </c>
+      <c r="B31" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="9"/>
     </row>
     <row r="32" ht="14.25">
       <c r="A32" s="6">
         <v>18</v>
       </c>
-      <c r="B32" t="s">
-        <v>58</v>
-      </c>
+      <c r="B32" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="9"/>
     </row>
     <row r="33" ht="14.25">
       <c r="A33" s="6">
         <v>19</v>
       </c>
-      <c r="B33" t="s">
-        <v>59</v>
-      </c>
+      <c r="B33" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="9"/>
     </row>
     <row r="34" ht="14.25">
       <c r="A34" s="6"/>
@@ -1407,6 +1746,27 @@
       <c r="A37" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="19">
+    <mergeCell ref="B15:I15"/>
+    <mergeCell ref="B16:I16"/>
+    <mergeCell ref="B17:I17"/>
+    <mergeCell ref="B18:I18"/>
+    <mergeCell ref="B19:I19"/>
+    <mergeCell ref="B20:I20"/>
+    <mergeCell ref="B21:I21"/>
+    <mergeCell ref="B22:I22"/>
+    <mergeCell ref="B23:I23"/>
+    <mergeCell ref="B24:I24"/>
+    <mergeCell ref="B25:I25"/>
+    <mergeCell ref="B26:I26"/>
+    <mergeCell ref="B27:I27"/>
+    <mergeCell ref="B28:I28"/>
+    <mergeCell ref="B29:I29"/>
+    <mergeCell ref="B30:I30"/>
+    <mergeCell ref="B31:I31"/>
+    <mergeCell ref="B32:I32"/>
+    <mergeCell ref="B33:I33"/>
+  </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>

</xml_diff>

<commit_message>
Progetto linguaggi a, completato parser e parsing
</commit_message>
<xml_diff>
--- a/Bruniera/linguaggi e compilatori/progetto/parteA/tabella2.xlsx
+++ b/Bruniera/linguaggi e compilatori/progetto/parteA/tabella2.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>NT\la</t>
   </si>
@@ -69,9 +69,6 @@
     <t>A'-&gt;EA''</t>
   </si>
   <si>
-    <t>A'-&gt;E,A''</t>
-  </si>
-  <si>
     <t>A''</t>
   </si>
   <si>
@@ -102,10 +99,10 @@
     <t>E</t>
   </si>
   <si>
-    <t xml:space="preserve">E-&gt; idE'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E-&gt; numE'</t>
+    <t xml:space="preserve">E-&gt; id E'</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E-&gt; num E'</t>
   </si>
   <si>
     <t>E'</t>
@@ -271,7 +268,7 @@
   <cellStyleXfs count="1">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="11">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
     <xf fontId="1" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -283,10 +280,6 @@
     <xf fontId="4" fillId="0" borderId="1" numFmtId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -801,6 +794,7 @@
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col customWidth="1" min="8" max="8" width="9.7109375"/>
+    <col customWidth="1" min="11" max="11" width="9.57421875"/>
     <col customWidth="1" min="13" max="13" width="11.421875"/>
   </cols>
   <sheetData>
@@ -917,14 +911,14 @@
       <c r="H3" s="6">
         <v>10</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="5" t="s">
         <v>17</v>
       </c>
       <c r="J3" s="4">
         <v>12</v>
       </c>
       <c r="K3" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="L3" s="6">
         <v>10</v>
@@ -938,19 +932,19 @@
     </row>
     <row r="4" ht="14.25">
       <c r="A4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="4">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="B4" s="4">
-        <v>3</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>20</v>
       </c>
       <c r="D4" s="4">
         <v>4</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4" s="4">
         <v>6</v>
@@ -958,8 +952,8 @@
       <c r="G4" s="4">
         <v>6</v>
       </c>
-      <c r="H4" s="7" t="s">
-        <v>20</v>
+      <c r="H4" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="I4" s="4">
         <v>11</v>
@@ -970,55 +964,55 @@
       <c r="K4" s="4">
         <v>11</v>
       </c>
-      <c r="L4" s="7" t="s">
-        <v>20</v>
+      <c r="L4" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="M4" s="4">
         <v>6</v>
       </c>
-      <c r="N4" s="7" t="s">
-        <v>20</v>
+      <c r="N4" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" ht="14.25">
       <c r="A5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="4">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4">
+        <v>2</v>
+      </c>
+      <c r="D5" s="4">
+        <v>2</v>
+      </c>
+      <c r="E5" s="4">
+        <v>2</v>
+      </c>
+      <c r="F5" s="4">
+        <v>2</v>
+      </c>
+      <c r="G5" s="4">
+        <v>2</v>
+      </c>
+      <c r="H5" s="4">
+        <v>2</v>
+      </c>
+      <c r="I5" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="4">
-        <v>2</v>
-      </c>
-      <c r="C5" s="4">
-        <v>2</v>
-      </c>
-      <c r="D5" s="4">
-        <v>2</v>
-      </c>
-      <c r="E5" s="4">
-        <v>2</v>
-      </c>
-      <c r="F5" s="4">
-        <v>2</v>
-      </c>
-      <c r="G5" s="4">
-        <v>2</v>
-      </c>
-      <c r="H5" s="4">
-        <v>2</v>
-      </c>
-      <c r="I5" s="5" t="s">
+      <c r="J5" s="4">
+        <v>2</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="L5" s="4">
+        <v>2</v>
+      </c>
+      <c r="M5" s="5" t="s">
         <v>23</v>
-      </c>
-      <c r="J5" s="4">
-        <v>2</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="L5" s="4">
-        <v>2</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>24</v>
       </c>
       <c r="N5" s="4">
         <v>1</v>
@@ -1026,7 +1020,7 @@
     </row>
     <row r="6" ht="14.25">
       <c r="A6" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" s="4">
         <v>3</v>
@@ -1041,10 +1035,10 @@
         <v>3</v>
       </c>
       <c r="F6" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="H6" s="4">
         <v>8</v>
@@ -1070,7 +1064,7 @@
     </row>
     <row r="7" ht="14.25">
       <c r="A7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="4">
         <v>3</v>
@@ -1093,14 +1087,14 @@
       <c r="H7" s="4">
         <v>16</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="4">
+        <v>3</v>
+      </c>
+      <c r="K7" s="7" t="s">
         <v>29</v>
-      </c>
-      <c r="J7" s="4">
-        <v>3</v>
-      </c>
-      <c r="K7" s="5" t="s">
-        <v>30</v>
       </c>
       <c r="L7" s="4">
         <v>16</v>
@@ -1114,28 +1108,28 @@
     </row>
     <row r="8" ht="14.25">
       <c r="A8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="4">
+        <v>3</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="4">
-        <v>3</v>
-      </c>
-      <c r="C8" s="5" t="s">
+      <c r="D8" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>33</v>
-      </c>
       <c r="E8" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I8" s="4">
         <v>15</v>
@@ -1147,21 +1141,21 @@
         <v>15</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="M8" s="4">
         <v>3</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="9" ht="14.25">
       <c r="A9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>34</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>35</v>
       </c>
       <c r="C9" s="4">
         <v>3</v>
@@ -1182,19 +1176,19 @@
         <v>7</v>
       </c>
       <c r="I9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="J9" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="J9" s="5" t="s">
-        <v>37</v>
-      </c>
       <c r="K9" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L9" s="4">
         <v>7</v>
       </c>
       <c r="M9" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="N9" s="4">
         <v>1</v>
@@ -1202,13 +1196,13 @@
     </row>
     <row r="10" ht="14.25">
       <c r="A10" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B10" s="4">
         <v>19</v>
       </c>
       <c r="C10" s="4">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="D10" s="4">
         <v>19</v>
@@ -1222,8 +1216,8 @@
       <c r="G10" s="4">
         <v>19</v>
       </c>
-      <c r="H10" s="7" t="s">
-        <v>39</v>
+      <c r="H10" s="5" t="s">
+        <v>38</v>
       </c>
       <c r="I10" s="4">
         <v>19</v>
@@ -1235,7 +1229,7 @@
         <v>19</v>
       </c>
       <c r="L10" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M10" s="4">
         <v>19</v>
@@ -1249,7 +1243,7 @@
     <row r="13" ht="14.25"/>
     <row r="14" ht="14.25">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" ht="15.6" customHeight="1">
@@ -1257,7 +1251,7 @@
         <v>1</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
@@ -1267,26 +1261,26 @@
       <c r="H15" s="9"/>
       <c r="I15" s="9"/>
       <c r="K15" s="10"/>
-      <c r="L15" s="11"/>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="11"/>
-      <c r="R15" s="11"/>
-      <c r="S15" s="11"/>
-      <c r="T15" s="11"/>
-      <c r="U15" s="11"/>
-      <c r="V15" s="11"/>
-      <c r="W15" s="11"/>
-      <c r="X15" s="11"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
     </row>
     <row r="16" ht="14.25">
       <c r="A16" s="6">
         <v>2</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
@@ -1296,26 +1290,26 @@
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
       <c r="K16" s="10"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="13"/>
-      <c r="N16" s="13"/>
-      <c r="O16" s="13"/>
-      <c r="P16" s="13"/>
-      <c r="Q16" s="13"/>
-      <c r="R16" s="13"/>
-      <c r="S16" s="13"/>
-      <c r="T16" s="13"/>
-      <c r="U16" s="13"/>
-      <c r="V16" s="13"/>
-      <c r="W16" s="13"/>
-      <c r="X16" s="13"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="9"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="9"/>
+      <c r="V16" s="9"/>
+      <c r="W16" s="9"/>
+      <c r="X16" s="9"/>
     </row>
     <row r="17" ht="14.25">
       <c r="A17" s="6">
         <v>3</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
@@ -1325,26 +1319,26 @@
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="K17" s="10"/>
-      <c r="L17" s="13"/>
-      <c r="M17" s="12"/>
-      <c r="N17" s="13"/>
-      <c r="O17" s="13"/>
-      <c r="P17" s="13"/>
-      <c r="Q17" s="13"/>
-      <c r="R17" s="13"/>
-      <c r="S17" s="13"/>
-      <c r="T17" s="13"/>
-      <c r="U17" s="13"/>
-      <c r="V17" s="13"/>
-      <c r="W17" s="13"/>
-      <c r="X17" s="13"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="9"/>
+      <c r="V17" s="9"/>
+      <c r="W17" s="9"/>
+      <c r="X17" s="9"/>
     </row>
     <row r="18" ht="14.25">
       <c r="A18" s="6">
         <v>4</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
@@ -1354,26 +1348,26 @@
       <c r="H18" s="9"/>
       <c r="I18" s="9"/>
       <c r="K18" s="10"/>
-      <c r="L18" s="13"/>
-      <c r="M18" s="13"/>
-      <c r="N18" s="12"/>
-      <c r="O18" s="13"/>
-      <c r="P18" s="13"/>
-      <c r="Q18" s="13"/>
-      <c r="R18" s="13"/>
-      <c r="S18" s="13"/>
-      <c r="T18" s="13"/>
-      <c r="U18" s="13"/>
-      <c r="V18" s="13"/>
-      <c r="W18" s="13"/>
-      <c r="X18" s="13"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="9"/>
+      <c r="T18" s="9"/>
+      <c r="U18" s="9"/>
+      <c r="V18" s="9"/>
+      <c r="W18" s="9"/>
+      <c r="X18" s="9"/>
     </row>
     <row r="19" ht="14.25">
       <c r="A19" s="6">
         <v>5</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
@@ -1383,26 +1377,26 @@
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
       <c r="K19" s="10"/>
-      <c r="L19" s="13"/>
-      <c r="M19" s="13"/>
-      <c r="N19" s="13"/>
-      <c r="O19" s="12"/>
-      <c r="P19" s="13"/>
-      <c r="Q19" s="13"/>
-      <c r="R19" s="13"/>
-      <c r="S19" s="13"/>
-      <c r="T19" s="13"/>
-      <c r="U19" s="13"/>
-      <c r="V19" s="13"/>
-      <c r="W19" s="13"/>
-      <c r="X19" s="13"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="9"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="9"/>
+      <c r="X19" s="9"/>
     </row>
     <row r="20" ht="14.25">
       <c r="A20" s="6">
         <v>6</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
@@ -1412,55 +1406,55 @@
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
       <c r="K20" s="10"/>
-      <c r="L20" s="13"/>
-      <c r="M20" s="13"/>
-      <c r="N20" s="13"/>
-      <c r="O20" s="13"/>
-      <c r="P20" s="12"/>
-      <c r="Q20" s="13"/>
-      <c r="R20" s="13"/>
-      <c r="S20" s="13"/>
-      <c r="T20" s="13"/>
-      <c r="U20" s="13"/>
-      <c r="V20" s="13"/>
-      <c r="W20" s="13"/>
-      <c r="X20" s="13"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="6"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
+      <c r="T20" s="9"/>
+      <c r="U20" s="9"/>
+      <c r="V20" s="9"/>
+      <c r="W20" s="9"/>
+      <c r="X20" s="9"/>
     </row>
     <row r="21" ht="14.25">
       <c r="A21" s="6">
         <v>7</v>
       </c>
-      <c r="B21" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="14"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
+      <c r="B21" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
       <c r="K21" s="10"/>
-      <c r="L21" s="13"/>
-      <c r="M21" s="13"/>
-      <c r="N21" s="13"/>
-      <c r="O21" s="13"/>
-      <c r="P21" s="13"/>
-      <c r="Q21" s="12"/>
-      <c r="R21" s="13"/>
-      <c r="S21" s="13"/>
-      <c r="T21" s="13"/>
-      <c r="U21" s="13"/>
-      <c r="V21" s="13"/>
-      <c r="W21" s="13"/>
-      <c r="X21" s="13"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="9"/>
+      <c r="V21" s="9"/>
+      <c r="W21" s="9"/>
+      <c r="X21" s="9"/>
     </row>
     <row r="22" ht="14.25">
       <c r="A22" s="6">
         <v>8</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
@@ -1470,26 +1464,26 @@
       <c r="H22" s="9"/>
       <c r="I22" s="9"/>
       <c r="K22" s="10"/>
-      <c r="L22" s="13"/>
-      <c r="M22" s="13"/>
-      <c r="N22" s="13"/>
-      <c r="O22" s="13"/>
-      <c r="P22" s="13"/>
-      <c r="Q22" s="13"/>
-      <c r="R22" s="12"/>
-      <c r="S22" s="13"/>
-      <c r="T22" s="13"/>
-      <c r="U22" s="13"/>
-      <c r="V22" s="13"/>
-      <c r="W22" s="13"/>
-      <c r="X22" s="13"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="6"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
+      <c r="V22" s="9"/>
+      <c r="W22" s="9"/>
+      <c r="X22" s="9"/>
     </row>
     <row r="23" ht="14.25">
       <c r="A23" s="6">
         <v>9</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
@@ -1499,26 +1493,26 @@
       <c r="H23" s="9"/>
       <c r="I23" s="9"/>
       <c r="K23" s="10"/>
-      <c r="L23" s="13"/>
-      <c r="M23" s="13"/>
-      <c r="N23" s="13"/>
-      <c r="O23" s="13"/>
-      <c r="P23" s="13"/>
-      <c r="Q23" s="13"/>
-      <c r="R23" s="13"/>
-      <c r="S23" s="12"/>
-      <c r="T23" s="13"/>
-      <c r="U23" s="13"/>
-      <c r="V23" s="13"/>
-      <c r="W23" s="13"/>
-      <c r="X23" s="13"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
+      <c r="S23" s="6"/>
+      <c r="T23" s="9"/>
+      <c r="U23" s="9"/>
+      <c r="V23" s="9"/>
+      <c r="W23" s="9"/>
+      <c r="X23" s="9"/>
     </row>
     <row r="24" ht="14.25">
       <c r="A24" s="6">
         <v>10</v>
       </c>
       <c r="B24" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
@@ -1528,26 +1522,26 @@
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
       <c r="K24" s="10"/>
-      <c r="L24" s="13"/>
-      <c r="M24" s="13"/>
-      <c r="N24" s="13"/>
-      <c r="O24" s="13"/>
-      <c r="P24" s="13"/>
-      <c r="Q24" s="13"/>
-      <c r="R24" s="13"/>
-      <c r="S24" s="13"/>
-      <c r="T24" s="12"/>
-      <c r="U24" s="13"/>
-      <c r="V24" s="13"/>
-      <c r="W24" s="13"/>
-      <c r="X24" s="13"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="6"/>
+      <c r="U24" s="9"/>
+      <c r="V24" s="9"/>
+      <c r="W24" s="9"/>
+      <c r="X24" s="9"/>
     </row>
     <row r="25" ht="14.25">
       <c r="A25" s="6">
         <v>11</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
@@ -1557,26 +1551,26 @@
       <c r="H25" s="9"/>
       <c r="I25" s="9"/>
       <c r="K25" s="10"/>
-      <c r="L25" s="13"/>
-      <c r="M25" s="13"/>
-      <c r="N25" s="13"/>
-      <c r="O25" s="13"/>
-      <c r="P25" s="13"/>
-      <c r="Q25" s="13"/>
-      <c r="R25" s="13"/>
-      <c r="S25" s="13"/>
-      <c r="T25" s="13"/>
-      <c r="U25" s="12"/>
-      <c r="V25" s="13"/>
-      <c r="W25" s="13"/>
-      <c r="X25" s="13"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="9"/>
+      <c r="U25" s="6"/>
+      <c r="V25" s="9"/>
+      <c r="W25" s="9"/>
+      <c r="X25" s="9"/>
     </row>
     <row r="26" ht="14.25">
       <c r="A26" s="6">
         <v>12</v>
       </c>
       <c r="B26" s="9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
@@ -1586,26 +1580,26 @@
       <c r="H26" s="9"/>
       <c r="I26" s="9"/>
       <c r="K26" s="10"/>
-      <c r="L26" s="13"/>
-      <c r="M26" s="13"/>
-      <c r="N26" s="13"/>
-      <c r="O26" s="13"/>
-      <c r="P26" s="13"/>
-      <c r="Q26" s="13"/>
-      <c r="R26" s="13"/>
-      <c r="S26" s="13"/>
-      <c r="T26" s="13"/>
-      <c r="U26" s="13"/>
-      <c r="V26" s="12"/>
-      <c r="W26" s="13"/>
-      <c r="X26" s="13"/>
+      <c r="L26" s="9"/>
+      <c r="M26" s="9"/>
+      <c r="N26" s="9"/>
+      <c r="O26" s="9"/>
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="9"/>
+      <c r="S26" s="9"/>
+      <c r="T26" s="9"/>
+      <c r="U26" s="9"/>
+      <c r="V26" s="6"/>
+      <c r="W26" s="9"/>
+      <c r="X26" s="9"/>
     </row>
     <row r="27" ht="14.25">
       <c r="A27" s="6">
         <v>13</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
@@ -1615,26 +1609,26 @@
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
       <c r="K27" s="10"/>
-      <c r="L27" s="13"/>
-      <c r="M27" s="13"/>
-      <c r="N27" s="13"/>
-      <c r="O27" s="13"/>
-      <c r="P27" s="13"/>
-      <c r="Q27" s="13"/>
-      <c r="R27" s="13"/>
-      <c r="S27" s="13"/>
-      <c r="T27" s="13"/>
-      <c r="U27" s="13"/>
-      <c r="V27" s="13"/>
-      <c r="W27" s="12"/>
-      <c r="X27" s="13"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="9"/>
+      <c r="R27" s="9"/>
+      <c r="S27" s="9"/>
+      <c r="T27" s="9"/>
+      <c r="U27" s="9"/>
+      <c r="V27" s="9"/>
+      <c r="W27" s="6"/>
+      <c r="X27" s="9"/>
     </row>
     <row r="28" ht="14.25">
       <c r="A28" s="6">
         <v>14</v>
       </c>
       <c r="B28" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
@@ -1644,26 +1638,26 @@
       <c r="H28" s="9"/>
       <c r="I28" s="9"/>
       <c r="K28" s="10"/>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="13"/>
-      <c r="O28" s="13"/>
-      <c r="P28" s="13"/>
-      <c r="Q28" s="13"/>
-      <c r="R28" s="13"/>
-      <c r="S28" s="13"/>
-      <c r="T28" s="13"/>
-      <c r="U28" s="13"/>
-      <c r="V28" s="13"/>
-      <c r="W28" s="13"/>
-      <c r="X28" s="12"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="9"/>
+      <c r="S28" s="9"/>
+      <c r="T28" s="9"/>
+      <c r="U28" s="9"/>
+      <c r="V28" s="9"/>
+      <c r="W28" s="9"/>
+      <c r="X28" s="6"/>
     </row>
     <row r="29" ht="14.25">
       <c r="A29" s="6">
         <v>15</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
@@ -1678,7 +1672,7 @@
         <v>16</v>
       </c>
       <c r="B30" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
@@ -1693,7 +1687,7 @@
         <v>17</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
@@ -1708,7 +1702,7 @@
         <v>18</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
@@ -1723,7 +1717,7 @@
         <v>19</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>

</xml_diff>